<commit_message>
1. change columns of fleetScenarioSimu.xlsx to required columns
</commit_message>
<xml_diff>
--- a/data/fleetScenarioSimu.xlsx
+++ b/data/fleetScenarioSimu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vn274765\Desktop\Code\python\smartcharging\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vn274765\Desktop\Code\python\smartcharging-clone\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544C831C-54D2-4B05-87EB-DB913DEDF980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFFBBC64-7F38-4F54-810E-83573C679D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="165">
   <si>
     <t>session_start</t>
   </si>
@@ -346,15 +346,6 @@
     <t>01:50:43</t>
   </si>
   <si>
-    <t>capacity_nom_kWh</t>
-  </si>
-  <si>
-    <t>soc_init</t>
-  </si>
-  <si>
-    <t>arrival</t>
-  </si>
-  <si>
     <t>05:45:00</t>
   </si>
   <si>
@@ -469,9 +460,6 @@
     <t>17:45:00</t>
   </si>
   <si>
-    <t>departure</t>
-  </si>
-  <si>
     <t>08:45:00</t>
   </si>
   <si>
@@ -517,13 +505,16 @@
     <t>19:30:00</t>
   </si>
   <si>
-    <t>capacity</t>
-  </si>
-  <si>
-    <t>pmax</t>
-  </si>
-  <si>
-    <t>pmin</t>
+    <t>arrivalTime</t>
+  </si>
+  <si>
+    <t>departureTime</t>
+  </si>
+  <si>
+    <t>energyMax</t>
+  </si>
+  <si>
+    <t>powerNom</t>
   </si>
 </sst>
 </file>
@@ -880,28 +871,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L104"/>
+  <dimension ref="A1:I104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="15.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.77734375" customWidth="1"/>
-    <col min="4" max="4" width="14.44140625" customWidth="1"/>
-    <col min="5" max="5" width="14.77734375" customWidth="1"/>
-    <col min="6" max="6" width="17.77734375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" customWidth="1"/>
-    <col min="12" max="12" width="5" customWidth="1"/>
+    <col min="1" max="2" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" customWidth="1"/>
+    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -918,28 +906,19 @@
         <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>108</v>
+        <v>161</v>
       </c>
       <c r="G1" t="s">
-        <v>109</v>
+        <v>162</v>
       </c>
       <c r="H1" t="s">
-        <v>110</v>
+        <v>163</v>
       </c>
       <c r="I1" t="s">
-        <v>149</v>
-      </c>
-      <c r="J1" t="s">
-        <v>165</v>
-      </c>
-      <c r="K1" t="s">
-        <v>166</v>
-      </c>
-      <c r="L1" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>45684.23710648148</v>
       </c>
@@ -955,29 +934,20 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G2" t="s">
+        <v>126</v>
+      </c>
+      <c r="H2">
         <v>54.7</v>
       </c>
-      <c r="G2">
-        <v>0.68051371115173676</v>
-      </c>
-      <c r="H2" t="s">
-        <v>111</v>
-      </c>
-      <c r="I2" t="s">
-        <v>129</v>
-      </c>
-      <c r="J2">
-        <v>54.7</v>
-      </c>
-      <c r="K2">
+      <c r="I2">
         <v>20.52</v>
       </c>
-      <c r="L2">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>45684.25403935185</v>
       </c>
@@ -993,29 +963,20 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G3" t="s">
+        <v>124</v>
+      </c>
+      <c r="H3">
         <v>67.5</v>
       </c>
-      <c r="G3">
-        <v>0.70930814814814813</v>
-      </c>
-      <c r="H3" t="s">
-        <v>112</v>
-      </c>
-      <c r="I3" t="s">
-        <v>127</v>
-      </c>
-      <c r="J3">
-        <v>67.5</v>
-      </c>
-      <c r="K3">
+      <c r="I3">
         <v>11.523999999999999</v>
       </c>
-      <c r="L3">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>45684.261608796296</v>
       </c>
@@ -1031,29 +992,20 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4">
+      <c r="F4" t="s">
+        <v>110</v>
+      </c>
+      <c r="G4" t="s">
+        <v>130</v>
+      </c>
+      <c r="H4">
         <v>69.900000000000006</v>
       </c>
-      <c r="G4">
-        <v>0.42044349070100145</v>
-      </c>
-      <c r="H4" t="s">
-        <v>113</v>
-      </c>
-      <c r="I4" t="s">
-        <v>133</v>
-      </c>
-      <c r="J4">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K4">
+      <c r="I4">
         <v>10.53</v>
       </c>
-      <c r="L4">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>45684.263090277775</v>
       </c>
@@ -1069,29 +1021,20 @@
       <c r="E5" t="s">
         <v>8</v>
       </c>
-      <c r="F5">
+      <c r="F5" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" t="s">
+        <v>141</v>
+      </c>
+      <c r="H5">
         <v>90</v>
       </c>
-      <c r="G5">
-        <v>0.76630222222222222</v>
-      </c>
-      <c r="H5" t="s">
-        <v>113</v>
-      </c>
-      <c r="I5" t="s">
-        <v>144</v>
-      </c>
-      <c r="J5">
-        <v>90</v>
-      </c>
-      <c r="K5">
+      <c r="I5">
         <v>8.6460000000000008</v>
       </c>
-      <c r="L5">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>45684.265208333331</v>
       </c>
@@ -1107,29 +1050,20 @@
       <c r="E6" t="s">
         <v>9</v>
       </c>
-      <c r="F6">
+      <c r="F6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G6" t="s">
+        <v>129</v>
+      </c>
+      <c r="H6">
         <v>67.5</v>
       </c>
-      <c r="G6">
-        <v>0.35364148148148156</v>
-      </c>
-      <c r="H6" t="s">
-        <v>113</v>
-      </c>
-      <c r="I6" t="s">
-        <v>132</v>
-      </c>
-      <c r="J6">
-        <v>67.5</v>
-      </c>
-      <c r="K6">
+      <c r="I6">
         <v>10.731999999999999</v>
       </c>
-      <c r="L6">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>45684.267974537041</v>
       </c>
@@ -1145,29 +1079,20 @@
       <c r="E7" t="s">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s">
+        <v>123</v>
+      </c>
+      <c r="H7">
         <v>78.099999999999994</v>
       </c>
-      <c r="G7">
-        <v>0.39669654289372602</v>
-      </c>
-      <c r="H7" t="s">
-        <v>114</v>
-      </c>
-      <c r="I7" t="s">
-        <v>126</v>
-      </c>
-      <c r="J7">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K7">
+      <c r="I7">
         <v>11.959</v>
       </c>
-      <c r="L7">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>45684.268460648149</v>
       </c>
@@ -1183,29 +1108,20 @@
       <c r="E8" t="s">
         <v>11</v>
       </c>
-      <c r="F8">
+      <c r="F8" t="s">
+        <v>111</v>
+      </c>
+      <c r="G8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8">
         <v>55.672777777777775</v>
       </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" t="s">
-        <v>126</v>
-      </c>
-      <c r="J8">
-        <v>55.672777777777775</v>
-      </c>
-      <c r="K8">
+      <c r="I8">
         <v>21.661999999999999</v>
       </c>
-      <c r="L8">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>45684.268460648149</v>
       </c>
@@ -1221,29 +1137,20 @@
       <c r="E9" t="s">
         <v>12</v>
       </c>
-      <c r="F9">
+      <c r="F9" t="s">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H9">
         <v>61.1</v>
       </c>
-      <c r="G9">
-        <v>0.34418821603927996</v>
-      </c>
-      <c r="H9" t="s">
-        <v>114</v>
-      </c>
-      <c r="I9" t="s">
-        <v>126</v>
-      </c>
-      <c r="J9">
-        <v>61.1</v>
-      </c>
-      <c r="K9">
+      <c r="I9">
         <v>10.608000000000001</v>
       </c>
-      <c r="L9">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>45684.269097222219</v>
       </c>
@@ -1259,29 +1166,20 @@
       <c r="E10" t="s">
         <v>13</v>
       </c>
-      <c r="F10">
+      <c r="F10" t="s">
+        <v>111</v>
+      </c>
+      <c r="G10" t="s">
+        <v>146</v>
+      </c>
+      <c r="H10">
         <v>90</v>
       </c>
-      <c r="G10">
-        <v>0.74340444444444442</v>
-      </c>
-      <c r="H10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I10" t="s">
-        <v>150</v>
-      </c>
-      <c r="J10">
-        <v>90</v>
-      </c>
-      <c r="K10">
+      <c r="I10">
         <v>7.3479999999999999</v>
       </c>
-      <c r="L10">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>45684.270277777781</v>
       </c>
@@ -1297,29 +1195,20 @@
       <c r="E11" t="s">
         <v>14</v>
       </c>
-      <c r="F11">
+      <c r="F11" t="s">
+        <v>111</v>
+      </c>
+      <c r="G11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H11">
         <v>90</v>
       </c>
-      <c r="G11">
-        <v>0.72582111111111114</v>
-      </c>
-      <c r="H11" t="s">
-        <v>114</v>
-      </c>
-      <c r="I11" t="s">
-        <v>127</v>
-      </c>
-      <c r="J11">
-        <v>90</v>
-      </c>
-      <c r="K11">
+      <c r="I11">
         <v>7.5030000000000001</v>
       </c>
-      <c r="L11">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>45684.271087962959</v>
       </c>
@@ -1335,29 +1224,20 @@
       <c r="E12" t="s">
         <v>15</v>
       </c>
-      <c r="F12">
+      <c r="F12" t="s">
+        <v>111</v>
+      </c>
+      <c r="G12" t="s">
+        <v>127</v>
+      </c>
+      <c r="H12">
         <v>49.432555555555552</v>
       </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12" t="s">
-        <v>114</v>
-      </c>
-      <c r="I12" t="s">
-        <v>130</v>
-      </c>
-      <c r="J12">
-        <v>49.432555555555552</v>
-      </c>
-      <c r="K12">
+      <c r="I12">
         <v>21.614999999999998</v>
       </c>
-      <c r="L12">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>45684.271747685183</v>
       </c>
@@ -1373,29 +1253,20 @@
       <c r="E13" t="s">
         <v>16</v>
       </c>
-      <c r="F13">
+      <c r="F13" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="H13">
         <v>36</v>
       </c>
-      <c r="G13">
-        <v>0.15832500000000005</v>
-      </c>
-      <c r="H13" t="s">
-        <v>114</v>
-      </c>
-      <c r="I13" t="s">
-        <v>133</v>
-      </c>
-      <c r="J13">
-        <v>36</v>
-      </c>
-      <c r="K13">
+      <c r="I13">
         <v>7.24</v>
       </c>
-      <c r="L13">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>45684.273217592592</v>
       </c>
@@ -1411,29 +1282,20 @@
       <c r="E14" t="s">
         <v>17</v>
       </c>
-      <c r="F14">
+      <c r="F14" t="s">
+        <v>111</v>
+      </c>
+      <c r="G14" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14">
         <v>90</v>
       </c>
-      <c r="G14">
-        <v>0.70342111111111116</v>
-      </c>
-      <c r="H14" t="s">
-        <v>114</v>
-      </c>
-      <c r="I14" t="s">
-        <v>132</v>
-      </c>
-      <c r="J14">
-        <v>90</v>
-      </c>
-      <c r="K14">
+      <c r="I14">
         <v>7.6260000000000003</v>
       </c>
-      <c r="L14">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>45684.274027777778</v>
       </c>
@@ -1449,29 +1311,20 @@
       <c r="E15" t="s">
         <v>18</v>
       </c>
-      <c r="F15">
+      <c r="F15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G15" t="s">
+        <v>120</v>
+      </c>
+      <c r="H15">
         <v>40</v>
       </c>
-      <c r="G15">
-        <v>0.52170500000000009</v>
-      </c>
-      <c r="H15" t="s">
-        <v>114</v>
-      </c>
-      <c r="I15" t="s">
-        <v>123</v>
-      </c>
-      <c r="J15">
-        <v>40</v>
-      </c>
-      <c r="K15">
+      <c r="I15">
         <v>6.8449999999999998</v>
       </c>
-      <c r="L15">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>45684.275960648149</v>
       </c>
@@ -1487,29 +1340,20 @@
       <c r="E16" t="s">
         <v>19</v>
       </c>
-      <c r="F16">
+      <c r="F16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" t="s">
+        <v>141</v>
+      </c>
+      <c r="H16">
         <v>70.915111111111102</v>
       </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16" t="s">
-        <v>114</v>
-      </c>
-      <c r="I16" t="s">
-        <v>144</v>
-      </c>
-      <c r="J16">
-        <v>70.915111111111102</v>
-      </c>
-      <c r="K16">
+      <c r="I16">
         <v>11.481</v>
       </c>
-      <c r="L16">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>45684.277465277781</v>
       </c>
@@ -1525,29 +1369,20 @@
       <c r="E17" t="s">
         <v>20</v>
       </c>
-      <c r="F17">
+      <c r="F17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17">
         <v>90</v>
       </c>
-      <c r="G17">
-        <v>0.8582144444444445</v>
-      </c>
-      <c r="H17" t="s">
-        <v>115</v>
-      </c>
-      <c r="I17" t="s">
-        <v>117</v>
-      </c>
-      <c r="J17">
-        <v>90</v>
-      </c>
-      <c r="K17">
+      <c r="I17">
         <v>7.6920000000000002</v>
       </c>
-      <c r="L17">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>45684.278009259258</v>
       </c>
@@ -1563,29 +1398,20 @@
       <c r="E18" t="s">
         <v>21</v>
       </c>
-      <c r="F18">
+      <c r="F18" t="s">
+        <v>112</v>
+      </c>
+      <c r="G18" t="s">
+        <v>147</v>
+      </c>
+      <c r="H18">
         <v>90</v>
       </c>
-      <c r="G18">
-        <v>0.61929888888888884</v>
-      </c>
-      <c r="H18" t="s">
-        <v>115</v>
-      </c>
-      <c r="I18" t="s">
-        <v>151</v>
-      </c>
-      <c r="J18">
-        <v>90</v>
-      </c>
-      <c r="K18">
+      <c r="I18">
         <v>7.2809999999999997</v>
       </c>
-      <c r="L18">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>45684.27815972222</v>
       </c>
@@ -1601,29 +1427,20 @@
       <c r="E19" t="s">
         <v>22</v>
       </c>
-      <c r="F19">
+      <c r="F19" t="s">
+        <v>112</v>
+      </c>
+      <c r="G19" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19">
         <v>82</v>
       </c>
-      <c r="G19">
-        <v>0.34537195121951225</v>
-      </c>
-      <c r="H19" t="s">
-        <v>115</v>
-      </c>
-      <c r="I19" t="s">
-        <v>132</v>
-      </c>
-      <c r="J19">
-        <v>82</v>
-      </c>
-      <c r="K19">
+      <c r="I19">
         <v>11.561999999999999</v>
       </c>
-      <c r="L19">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>45684.279085648152</v>
       </c>
@@ -1639,29 +1456,20 @@
       <c r="E20" t="s">
         <v>23</v>
       </c>
-      <c r="F20">
+      <c r="F20" t="s">
+        <v>112</v>
+      </c>
+      <c r="G20" t="s">
+        <v>140</v>
+      </c>
+      <c r="H20">
         <v>90</v>
       </c>
-      <c r="G20">
-        <v>0.6464011111111112</v>
-      </c>
-      <c r="H20" t="s">
-        <v>115</v>
-      </c>
-      <c r="I20" t="s">
-        <v>143</v>
-      </c>
-      <c r="J20">
-        <v>90</v>
-      </c>
-      <c r="K20">
+      <c r="I20">
         <v>7.3010000000000002</v>
       </c>
-      <c r="L20">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>45684.279942129629</v>
       </c>
@@ -1677,29 +1485,20 @@
       <c r="E21" t="s">
         <v>24</v>
       </c>
-      <c r="F21">
+      <c r="F21" t="s">
+        <v>112</v>
+      </c>
+      <c r="G21" t="s">
+        <v>139</v>
+      </c>
+      <c r="H21">
         <v>82</v>
       </c>
-      <c r="G21">
-        <v>0.71300000000000008</v>
-      </c>
-      <c r="H21" t="s">
-        <v>115</v>
-      </c>
-      <c r="I21" t="s">
-        <v>142</v>
-      </c>
-      <c r="J21">
-        <v>82</v>
-      </c>
-      <c r="K21">
+      <c r="I21">
         <v>11.004</v>
       </c>
-      <c r="L21">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>45684.280972222223</v>
       </c>
@@ -1715,29 +1514,20 @@
       <c r="E22" t="s">
         <v>25</v>
       </c>
-      <c r="F22">
+      <c r="F22" t="s">
+        <v>112</v>
+      </c>
+      <c r="G22" t="s">
+        <v>123</v>
+      </c>
+      <c r="H22">
         <v>40</v>
       </c>
-      <c r="G22">
-        <v>0.2617775</v>
-      </c>
-      <c r="H22" t="s">
-        <v>115</v>
-      </c>
-      <c r="I22" t="s">
-        <v>126</v>
-      </c>
-      <c r="J22">
-        <v>40</v>
-      </c>
-      <c r="K22">
+      <c r="I22">
         <v>6.8410000000000002</v>
       </c>
-      <c r="L22">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>45684.2815162037</v>
       </c>
@@ -1753,29 +1543,20 @@
       <c r="E23" t="s">
         <v>26</v>
       </c>
-      <c r="F23">
+      <c r="F23" t="s">
+        <v>112</v>
+      </c>
+      <c r="G23" t="s">
+        <v>125</v>
+      </c>
+      <c r="H23">
         <v>90</v>
       </c>
-      <c r="G23">
-        <v>0.64180999999999999</v>
-      </c>
-      <c r="H23" t="s">
-        <v>115</v>
-      </c>
-      <c r="I23" t="s">
-        <v>128</v>
-      </c>
-      <c r="J23">
-        <v>90</v>
-      </c>
-      <c r="K23">
+      <c r="I23">
         <v>7.3410000000000002</v>
       </c>
-      <c r="L23">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>45684.281990740739</v>
       </c>
@@ -1791,29 +1572,20 @@
       <c r="E24" t="s">
         <v>27</v>
       </c>
-      <c r="F24">
+      <c r="F24" t="s">
+        <v>112</v>
+      </c>
+      <c r="G24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H24">
         <v>78.099999999999994</v>
       </c>
-      <c r="G24">
-        <v>0.62688988476312424</v>
-      </c>
-      <c r="H24" t="s">
-        <v>115</v>
-      </c>
-      <c r="I24" t="s">
-        <v>124</v>
-      </c>
-      <c r="J24">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K24">
+      <c r="I24">
         <v>13.654</v>
       </c>
-      <c r="L24">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>45684.283229166664</v>
       </c>
@@ -1829,29 +1601,20 @@
       <c r="E25" t="s">
         <v>28</v>
       </c>
-      <c r="F25">
+      <c r="F25" t="s">
+        <v>112</v>
+      </c>
+      <c r="G25" t="s">
+        <v>129</v>
+      </c>
+      <c r="H25">
         <v>62</v>
       </c>
-      <c r="G25">
-        <v>8.6722580645161251E-2</v>
-      </c>
-      <c r="H25" t="s">
-        <v>115</v>
-      </c>
-      <c r="I25" t="s">
-        <v>132</v>
-      </c>
-      <c r="J25">
-        <v>62</v>
-      </c>
-      <c r="K25">
+      <c r="I25">
         <v>11.291</v>
       </c>
-      <c r="L25">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>45684.284097222226</v>
       </c>
@@ -1867,29 +1630,20 @@
       <c r="E26" t="s">
         <v>29</v>
       </c>
-      <c r="F26">
+      <c r="F26" t="s">
+        <v>112</v>
+      </c>
+      <c r="G26" t="s">
+        <v>123</v>
+      </c>
+      <c r="H26">
         <v>54.7</v>
       </c>
-      <c r="G26">
-        <v>0.26666179159049364</v>
-      </c>
-      <c r="H26" t="s">
-        <v>115</v>
-      </c>
-      <c r="I26" t="s">
-        <v>126</v>
-      </c>
-      <c r="J26">
-        <v>54.7</v>
-      </c>
-      <c r="K26">
+      <c r="I26">
         <v>19.928999999999998</v>
       </c>
-      <c r="L26">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>45684.28979166667</v>
       </c>
@@ -1905,29 +1659,20 @@
       <c r="E27" t="s">
         <v>30</v>
       </c>
-      <c r="F27">
+      <c r="F27" t="s">
+        <v>113</v>
+      </c>
+      <c r="G27" t="s">
+        <v>125</v>
+      </c>
+      <c r="H27">
         <v>69.900000000000006</v>
       </c>
-      <c r="G27">
-        <v>0.52249213161659513</v>
-      </c>
-      <c r="H27" t="s">
-        <v>116</v>
-      </c>
-      <c r="I27" t="s">
-        <v>128</v>
-      </c>
-      <c r="J27">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K27">
+      <c r="I27">
         <v>10.510999999999999</v>
       </c>
-      <c r="L27">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>45684.291354166664</v>
       </c>
@@ -1943,29 +1688,20 @@
       <c r="E28" t="s">
         <v>31</v>
       </c>
-      <c r="F28">
+      <c r="F28" t="s">
+        <v>113</v>
+      </c>
+      <c r="G28" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28">
         <v>65</v>
       </c>
-      <c r="G28">
-        <v>0.51402000000000003</v>
-      </c>
-      <c r="H28" t="s">
-        <v>116</v>
-      </c>
-      <c r="I28" t="s">
-        <v>134</v>
-      </c>
-      <c r="J28">
-        <v>65</v>
-      </c>
-      <c r="K28">
+      <c r="I28">
         <v>11.13</v>
       </c>
-      <c r="L28">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>45684.291597222225</v>
       </c>
@@ -1981,29 +1717,20 @@
       <c r="E29" t="s">
         <v>32</v>
       </c>
-      <c r="F29">
+      <c r="F29" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29">
         <v>90</v>
       </c>
-      <c r="G29">
-        <v>0.40843555555555555</v>
-      </c>
-      <c r="H29" t="s">
-        <v>116</v>
-      </c>
-      <c r="I29" t="s">
-        <v>137</v>
-      </c>
-      <c r="J29">
-        <v>90</v>
-      </c>
-      <c r="K29">
+      <c r="I29">
         <v>7.5279999999999996</v>
       </c>
-      <c r="L29">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>45684.291747685187</v>
       </c>
@@ -2019,29 +1746,20 @@
       <c r="E30" t="s">
         <v>33</v>
       </c>
-      <c r="F30">
+      <c r="F30" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" t="s">
+        <v>126</v>
+      </c>
+      <c r="H30">
         <v>82</v>
       </c>
-      <c r="G30">
-        <v>0.40776585365853663</v>
-      </c>
-      <c r="H30" t="s">
-        <v>116</v>
-      </c>
-      <c r="I30" t="s">
-        <v>129</v>
-      </c>
-      <c r="J30">
-        <v>82</v>
-      </c>
-      <c r="K30">
+      <c r="I30">
         <v>10.984999999999999</v>
       </c>
-      <c r="L30">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>45684.292731481481</v>
       </c>
@@ -2057,29 +1775,20 @@
       <c r="E31" t="s">
         <v>34</v>
       </c>
-      <c r="F31">
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+      <c r="G31" t="s">
+        <v>129</v>
+      </c>
+      <c r="H31">
         <v>54.7</v>
       </c>
-      <c r="G31">
-        <v>0.63897257769652649</v>
-      </c>
-      <c r="H31" t="s">
-        <v>116</v>
-      </c>
-      <c r="I31" t="s">
-        <v>132</v>
-      </c>
-      <c r="J31">
-        <v>54.7</v>
-      </c>
-      <c r="K31">
+      <c r="I31">
         <v>20.757999999999999</v>
       </c>
-      <c r="L31">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>45684.293287037035</v>
       </c>
@@ -2095,29 +1804,20 @@
       <c r="E32" t="s">
         <v>35</v>
       </c>
-      <c r="F32">
+      <c r="F32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G32" t="s">
+        <v>148</v>
+      </c>
+      <c r="H32">
         <v>69.900000000000006</v>
       </c>
-      <c r="G32">
-        <v>0.74388984263233193</v>
-      </c>
-      <c r="H32" t="s">
-        <v>116</v>
-      </c>
-      <c r="I32" t="s">
-        <v>152</v>
-      </c>
-      <c r="J32">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K32">
+      <c r="I32">
         <v>10.448</v>
       </c>
-      <c r="L32">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>45684.298472222225</v>
       </c>
@@ -2133,29 +1833,20 @@
       <c r="E33" t="s">
         <v>36</v>
       </c>
-      <c r="F33">
+      <c r="F33" t="s">
+        <v>114</v>
+      </c>
+      <c r="G33" t="s">
+        <v>134</v>
+      </c>
+      <c r="H33">
         <v>90</v>
       </c>
-      <c r="G33">
-        <v>0.67964888888888886</v>
-      </c>
-      <c r="H33" t="s">
-        <v>117</v>
-      </c>
-      <c r="I33" t="s">
-        <v>137</v>
-      </c>
-      <c r="J33">
-        <v>90</v>
-      </c>
-      <c r="K33">
+      <c r="I33">
         <v>7.6050000000000004</v>
       </c>
-      <c r="L33">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>45684.300995370373</v>
       </c>
@@ -2171,29 +1862,20 @@
       <c r="E34" t="s">
         <v>37</v>
       </c>
-      <c r="F34">
+      <c r="F34" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" t="s">
+        <v>132</v>
+      </c>
+      <c r="H34">
         <v>62</v>
       </c>
-      <c r="G34">
-        <v>0.16743225806451623</v>
-      </c>
-      <c r="H34" t="s">
-        <v>117</v>
-      </c>
-      <c r="I34" t="s">
-        <v>135</v>
-      </c>
-      <c r="J34">
-        <v>62</v>
-      </c>
-      <c r="K34">
+      <c r="I34">
         <v>11.285</v>
       </c>
-      <c r="L34">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>45684.301770833335</v>
       </c>
@@ -2209,29 +1891,20 @@
       <c r="E35" t="s">
         <v>38</v>
       </c>
-      <c r="F35">
+      <c r="F35" t="s">
+        <v>114</v>
+      </c>
+      <c r="G35" t="s">
+        <v>130</v>
+      </c>
+      <c r="H35">
         <v>90</v>
       </c>
-      <c r="G35">
-        <v>0.71717888888888892</v>
-      </c>
-      <c r="H35" t="s">
-        <v>117</v>
-      </c>
-      <c r="I35" t="s">
-        <v>133</v>
-      </c>
-      <c r="J35">
-        <v>90</v>
-      </c>
-      <c r="K35">
+      <c r="I35">
         <v>7.6760000000000002</v>
       </c>
-      <c r="L35">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>45684.302094907405</v>
       </c>
@@ -2247,29 +1920,20 @@
       <c r="E36" t="s">
         <v>39</v>
       </c>
-      <c r="F36">
+      <c r="F36" t="s">
+        <v>114</v>
+      </c>
+      <c r="G36" t="s">
+        <v>133</v>
+      </c>
+      <c r="H36">
         <v>54.7</v>
       </c>
-      <c r="G36">
-        <v>0.16900731261425961</v>
-      </c>
-      <c r="H36" t="s">
-        <v>117</v>
-      </c>
-      <c r="I36" t="s">
-        <v>136</v>
-      </c>
-      <c r="J36">
-        <v>54.7</v>
-      </c>
-      <c r="K36">
+      <c r="I36">
         <v>20.425999999999998</v>
       </c>
-      <c r="L36">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>45684.302164351851</v>
       </c>
@@ -2285,29 +1949,20 @@
       <c r="E37" t="s">
         <v>40</v>
       </c>
-      <c r="F37">
+      <c r="F37" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" t="s">
+        <v>123</v>
+      </c>
+      <c r="H37">
         <v>90</v>
       </c>
-      <c r="G37">
-        <v>0.7383588888888889</v>
-      </c>
-      <c r="H37" t="s">
-        <v>117</v>
-      </c>
-      <c r="I37" t="s">
-        <v>126</v>
-      </c>
-      <c r="J37">
-        <v>90</v>
-      </c>
-      <c r="K37">
+      <c r="I37">
         <v>7.84</v>
       </c>
-      <c r="L37">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>45684.302164351851</v>
       </c>
@@ -2323,29 +1978,20 @@
       <c r="E38" t="s">
         <v>41</v>
       </c>
-      <c r="F38">
+      <c r="F38" t="s">
+        <v>114</v>
+      </c>
+      <c r="G38" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38">
         <v>62</v>
       </c>
-      <c r="G38">
-        <v>0.67963064516129035</v>
-      </c>
-      <c r="H38" t="s">
-        <v>117</v>
-      </c>
-      <c r="I38" t="s">
-        <v>124</v>
-      </c>
-      <c r="J38">
-        <v>62</v>
-      </c>
-      <c r="K38">
+      <c r="I38">
         <v>6.7279999999999998</v>
       </c>
-      <c r="L38">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>45684.303402777776</v>
       </c>
@@ -2361,29 +2007,20 @@
       <c r="E39" t="s">
         <v>42</v>
       </c>
-      <c r="F39">
+      <c r="F39" t="s">
+        <v>114</v>
+      </c>
+      <c r="G39" t="s">
+        <v>126</v>
+      </c>
+      <c r="H39">
         <v>62</v>
       </c>
-      <c r="G39">
-        <v>0.78156451612903233</v>
-      </c>
-      <c r="H39" t="s">
-        <v>117</v>
-      </c>
-      <c r="I39" t="s">
-        <v>129</v>
-      </c>
-      <c r="J39">
-        <v>62</v>
-      </c>
-      <c r="K39">
+      <c r="I39">
         <v>10.946</v>
       </c>
-      <c r="L39">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>45684.309710648151</v>
       </c>
@@ -2399,29 +2036,20 @@
       <c r="E40" t="s">
         <v>43</v>
       </c>
-      <c r="F40">
+      <c r="F40" t="s">
+        <v>115</v>
+      </c>
+      <c r="G40" t="s">
+        <v>120</v>
+      </c>
+      <c r="H40">
         <v>36</v>
       </c>
-      <c r="G40">
-        <v>0.45400000000000001</v>
-      </c>
-      <c r="H40" t="s">
-        <v>118</v>
-      </c>
-      <c r="I40" t="s">
-        <v>123</v>
-      </c>
-      <c r="J40">
-        <v>36</v>
-      </c>
-      <c r="K40">
+      <c r="I40">
         <v>7.2229999999999999</v>
       </c>
-      <c r="L40">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>45684.313101851854</v>
       </c>
@@ -2437,29 +2065,20 @@
       <c r="E41" t="s">
         <v>44</v>
       </c>
-      <c r="F41">
+      <c r="F41" t="s">
+        <v>115</v>
+      </c>
+      <c r="G41" t="s">
+        <v>125</v>
+      </c>
+      <c r="H41">
         <v>90</v>
       </c>
-      <c r="G41">
-        <v>0.65766222222222226</v>
-      </c>
-      <c r="H41" t="s">
-        <v>118</v>
-      </c>
-      <c r="I41" t="s">
-        <v>128</v>
-      </c>
-      <c r="J41">
-        <v>90</v>
-      </c>
-      <c r="K41">
+      <c r="I41">
         <v>7.2889999999999997</v>
       </c>
-      <c r="L41">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>45684.313148148147</v>
       </c>
@@ -2475,29 +2094,20 @@
       <c r="E42" t="s">
         <v>45</v>
       </c>
-      <c r="F42">
+      <c r="F42" t="s">
+        <v>115</v>
+      </c>
+      <c r="G42" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42">
         <v>90</v>
       </c>
-      <c r="G42">
-        <v>0.81648777777777781</v>
-      </c>
-      <c r="H42" t="s">
-        <v>118</v>
-      </c>
-      <c r="I42" t="s">
-        <v>153</v>
-      </c>
-      <c r="J42">
-        <v>90</v>
-      </c>
-      <c r="K42">
+      <c r="I42">
         <v>7.3609999999999998</v>
       </c>
-      <c r="L42">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>45684.31322916667</v>
       </c>
@@ -2513,29 +2123,20 @@
       <c r="E43" t="s">
         <v>46</v>
       </c>
-      <c r="F43">
+      <c r="F43" t="s">
+        <v>115</v>
+      </c>
+      <c r="G43" t="s">
+        <v>150</v>
+      </c>
+      <c r="H43">
         <v>82</v>
       </c>
-      <c r="G43">
-        <v>0.40577926829268296</v>
-      </c>
-      <c r="H43" t="s">
-        <v>118</v>
-      </c>
-      <c r="I43" t="s">
-        <v>154</v>
-      </c>
-      <c r="J43">
-        <v>82</v>
-      </c>
-      <c r="K43">
+      <c r="I43">
         <v>11.528</v>
       </c>
-      <c r="L43">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>45684.315057870372</v>
       </c>
@@ -2551,29 +2152,20 @@
       <c r="E44" t="s">
         <v>47</v>
       </c>
-      <c r="F44">
+      <c r="F44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G44" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44">
         <v>78.099999999999994</v>
       </c>
-      <c r="G44">
-        <v>0.45992701664532648</v>
-      </c>
-      <c r="H44" t="s">
-        <v>118</v>
-      </c>
-      <c r="I44" t="s">
-        <v>137</v>
-      </c>
-      <c r="J44">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K44">
+      <c r="I44">
         <v>11.672000000000001</v>
       </c>
-      <c r="L44">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>45684.31658564815</v>
       </c>
@@ -2589,29 +2181,20 @@
       <c r="E45" t="s">
         <v>48</v>
       </c>
-      <c r="F45">
+      <c r="F45" t="s">
+        <v>115</v>
+      </c>
+      <c r="G45" t="s">
+        <v>124</v>
+      </c>
+      <c r="H45">
         <v>90</v>
       </c>
-      <c r="G45">
-        <v>0.66338444444444444</v>
-      </c>
-      <c r="H45" t="s">
-        <v>118</v>
-      </c>
-      <c r="I45" t="s">
-        <v>127</v>
-      </c>
-      <c r="J45">
-        <v>90</v>
-      </c>
-      <c r="K45">
+      <c r="I45">
         <v>7.3419999999999996</v>
       </c>
-      <c r="L45">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>45684.319571759261</v>
       </c>
@@ -2627,29 +2210,20 @@
       <c r="E46" t="s">
         <v>49</v>
       </c>
-      <c r="F46">
+      <c r="F46" t="s">
+        <v>116</v>
+      </c>
+      <c r="G46" t="s">
+        <v>118</v>
+      </c>
+      <c r="H46">
         <v>69</v>
       </c>
-      <c r="G46">
-        <v>0.77077391304347831</v>
-      </c>
-      <c r="H46" t="s">
-        <v>119</v>
-      </c>
-      <c r="I46" t="s">
-        <v>121</v>
-      </c>
-      <c r="J46">
-        <v>69</v>
-      </c>
-      <c r="K46">
+      <c r="I46">
         <v>11.097</v>
       </c>
-      <c r="L46">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45684.320844907408</v>
       </c>
@@ -2665,29 +2239,20 @@
       <c r="E47" t="s">
         <v>50</v>
       </c>
-      <c r="F47">
+      <c r="F47" t="s">
+        <v>116</v>
+      </c>
+      <c r="G47" t="s">
+        <v>119</v>
+      </c>
+      <c r="H47">
         <v>36</v>
       </c>
-      <c r="G47">
-        <v>0.61372222222222228</v>
-      </c>
-      <c r="H47" t="s">
-        <v>119</v>
-      </c>
-      <c r="I47" t="s">
-        <v>122</v>
-      </c>
-      <c r="J47">
-        <v>36</v>
-      </c>
-      <c r="K47">
+      <c r="I47">
         <v>7.1760000000000002</v>
       </c>
-      <c r="L47">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>45684.322928240741</v>
       </c>
@@ -2703,29 +2268,20 @@
       <c r="E48" t="s">
         <v>51</v>
       </c>
-      <c r="F48">
+      <c r="F48" t="s">
+        <v>116</v>
+      </c>
+      <c r="G48" t="s">
+        <v>133</v>
+      </c>
+      <c r="H48">
         <v>78.099999999999994</v>
       </c>
-      <c r="G48">
-        <v>0.40848015364916768</v>
-      </c>
-      <c r="H48" t="s">
-        <v>119</v>
-      </c>
-      <c r="I48" t="s">
-        <v>136</v>
-      </c>
-      <c r="J48">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K48">
+      <c r="I48">
         <v>11.75</v>
       </c>
-      <c r="L48">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>45684.32471064815</v>
       </c>
@@ -2741,29 +2297,20 @@
       <c r="E49" t="s">
         <v>52</v>
       </c>
-      <c r="F49">
+      <c r="F49" t="s">
+        <v>116</v>
+      </c>
+      <c r="G49" t="s">
+        <v>119</v>
+      </c>
+      <c r="H49">
         <v>90</v>
       </c>
-      <c r="G49">
-        <v>0.85322333333333333</v>
-      </c>
-      <c r="H49" t="s">
-        <v>119</v>
-      </c>
-      <c r="I49" t="s">
-        <v>122</v>
-      </c>
-      <c r="J49">
-        <v>90</v>
-      </c>
-      <c r="K49">
+      <c r="I49">
         <v>7.306</v>
       </c>
-      <c r="L49">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>45684.325671296298</v>
       </c>
@@ -2779,29 +2326,20 @@
       <c r="E50" t="s">
         <v>53</v>
       </c>
-      <c r="F50">
+      <c r="F50" t="s">
+        <v>116</v>
+      </c>
+      <c r="G50" t="s">
+        <v>128</v>
+      </c>
+      <c r="H50">
         <v>78.099999999999994</v>
       </c>
-      <c r="G50">
-        <v>0.5831306017925737</v>
-      </c>
-      <c r="H50" t="s">
-        <v>119</v>
-      </c>
-      <c r="I50" t="s">
-        <v>131</v>
-      </c>
-      <c r="J50">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K50">
+      <c r="I50">
         <v>11.72</v>
       </c>
-      <c r="L50">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>45684.343078703707</v>
       </c>
@@ -2817,29 +2355,20 @@
       <c r="E51" t="s">
         <v>54</v>
       </c>
-      <c r="F51">
+      <c r="F51" t="s">
+        <v>117</v>
+      </c>
+      <c r="G51" t="s">
+        <v>132</v>
+      </c>
+      <c r="H51">
         <v>78.099999999999994</v>
       </c>
-      <c r="G51">
-        <v>0.35880153649167734</v>
-      </c>
-      <c r="H51" t="s">
-        <v>120</v>
-      </c>
-      <c r="I51" t="s">
-        <v>135</v>
-      </c>
-      <c r="J51">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K51">
+      <c r="I51">
         <v>11.723000000000001</v>
       </c>
-      <c r="L51">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>45684.345300925925</v>
       </c>
@@ -2855,29 +2384,20 @@
       <c r="E52" t="s">
         <v>55</v>
       </c>
-      <c r="F52">
+      <c r="F52" t="s">
+        <v>117</v>
+      </c>
+      <c r="G52" t="s">
+        <v>123</v>
+      </c>
+      <c r="H52">
         <v>54.7</v>
       </c>
-      <c r="G52">
-        <v>0.13333272394881168</v>
-      </c>
-      <c r="H52" t="s">
-        <v>120</v>
-      </c>
-      <c r="I52" t="s">
-        <v>126</v>
-      </c>
-      <c r="J52">
-        <v>54.7</v>
-      </c>
-      <c r="K52">
+      <c r="I52">
         <v>20.431999999999999</v>
       </c>
-      <c r="L52">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>45684.358263888891</v>
       </c>
@@ -2893,29 +2413,20 @@
       <c r="E53" t="s">
         <v>56</v>
       </c>
-      <c r="F53">
+      <c r="F53" t="s">
+        <v>118</v>
+      </c>
+      <c r="G53" t="s">
+        <v>137</v>
+      </c>
+      <c r="H53">
         <v>69.900000000000006</v>
       </c>
-      <c r="G53">
-        <v>0.28296995708154515</v>
-      </c>
-      <c r="H53" t="s">
-        <v>121</v>
-      </c>
-      <c r="I53" t="s">
-        <v>140</v>
-      </c>
-      <c r="J53">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K53">
+      <c r="I53">
         <v>10.541</v>
       </c>
-      <c r="L53">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>45684.358402777776</v>
       </c>
@@ -2931,29 +2442,20 @@
       <c r="E54" t="s">
         <v>57</v>
       </c>
-      <c r="F54">
+      <c r="F54" t="s">
+        <v>118</v>
+      </c>
+      <c r="G54" t="s">
+        <v>149</v>
+      </c>
+      <c r="H54">
         <v>50</v>
       </c>
-      <c r="G54">
-        <v>0.82433400000000001</v>
-      </c>
-      <c r="H54" t="s">
-        <v>121</v>
-      </c>
-      <c r="I54" t="s">
-        <v>153</v>
-      </c>
-      <c r="J54">
-        <v>50</v>
-      </c>
-      <c r="K54">
+      <c r="I54">
         <v>9.98</v>
       </c>
-      <c r="L54">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>45684.39640046296</v>
       </c>
@@ -2969,29 +2471,20 @@
       <c r="E55" t="s">
         <v>58</v>
       </c>
-      <c r="F55">
+      <c r="F55" t="s">
+        <v>119</v>
+      </c>
+      <c r="G55" t="s">
+        <v>137</v>
+      </c>
+      <c r="H55">
         <v>69.900000000000006</v>
       </c>
-      <c r="G55">
-        <v>0.44654935622317599</v>
-      </c>
-      <c r="H55" t="s">
-        <v>122</v>
-      </c>
-      <c r="I55" t="s">
-        <v>140</v>
-      </c>
-      <c r="J55">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K55">
+      <c r="I55">
         <v>10.436</v>
       </c>
-      <c r="L55">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>45684.403414351851</v>
       </c>
@@ -3007,29 +2500,20 @@
       <c r="E56" t="s">
         <v>59</v>
       </c>
-      <c r="F56">
+      <c r="F56" t="s">
+        <v>120</v>
+      </c>
+      <c r="G56" t="s">
+        <v>125</v>
+      </c>
+      <c r="H56">
         <v>45</v>
       </c>
-      <c r="G56">
-        <v>0.47201777777777781</v>
-      </c>
-      <c r="H56" t="s">
-        <v>123</v>
-      </c>
-      <c r="I56" t="s">
-        <v>128</v>
-      </c>
-      <c r="J56">
-        <v>45</v>
-      </c>
-      <c r="K56">
+      <c r="I56">
         <v>20.989000000000001</v>
       </c>
-      <c r="L56">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>45684.408275462964</v>
       </c>
@@ -3045,29 +2529,20 @@
       <c r="E57" t="s">
         <v>60</v>
       </c>
-      <c r="F57">
+      <c r="F57" t="s">
+        <v>120</v>
+      </c>
+      <c r="G57" t="s">
+        <v>133</v>
+      </c>
+      <c r="H57">
         <v>69.900000000000006</v>
       </c>
-      <c r="G57">
-        <v>0.55611587982832622</v>
-      </c>
-      <c r="H57" t="s">
-        <v>123</v>
-      </c>
-      <c r="I57" t="s">
-        <v>136</v>
-      </c>
-      <c r="J57">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K57">
+      <c r="I57">
         <v>10.523</v>
       </c>
-      <c r="L57">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>45684.411249999997</v>
       </c>
@@ -3083,29 +2558,20 @@
       <c r="E58" t="s">
         <v>61</v>
       </c>
-      <c r="F58">
+      <c r="F58" t="s">
+        <v>120</v>
+      </c>
+      <c r="G58" t="s">
+        <v>127</v>
+      </c>
+      <c r="H58">
         <v>36</v>
       </c>
-      <c r="G58">
-        <v>0.60138333333333338</v>
-      </c>
-      <c r="H58" t="s">
-        <v>123</v>
-      </c>
-      <c r="I58" t="s">
-        <v>130</v>
-      </c>
-      <c r="J58">
-        <v>36</v>
-      </c>
-      <c r="K58">
+      <c r="I58">
         <v>7.2140000000000004</v>
       </c>
-      <c r="L58">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>45684.413321759261</v>
       </c>
@@ -3121,29 +2587,20 @@
       <c r="E59" t="s">
         <v>62</v>
       </c>
-      <c r="F59">
+      <c r="F59" t="s">
+        <v>121</v>
+      </c>
+      <c r="G59" t="s">
+        <v>151</v>
+      </c>
+      <c r="H59">
         <v>54.7</v>
       </c>
-      <c r="G59">
-        <v>0.69772760511883003</v>
-      </c>
-      <c r="H59" t="s">
-        <v>124</v>
-      </c>
-      <c r="I59" t="s">
-        <v>155</v>
-      </c>
-      <c r="J59">
-        <v>54.7</v>
-      </c>
-      <c r="K59">
+      <c r="I59">
         <v>20.82</v>
       </c>
-      <c r="L59">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>45684.422766203701</v>
       </c>
@@ -3159,29 +2616,20 @@
       <c r="E60" t="s">
         <v>63</v>
       </c>
-      <c r="F60">
+      <c r="F60" t="s">
+        <v>122</v>
+      </c>
+      <c r="G60" t="s">
+        <v>147</v>
+      </c>
+      <c r="H60">
         <v>36</v>
       </c>
-      <c r="G60">
-        <v>0.82854722222222221</v>
-      </c>
-      <c r="H60" t="s">
-        <v>125</v>
-      </c>
-      <c r="I60" t="s">
-        <v>151</v>
-      </c>
-      <c r="J60">
-        <v>36</v>
-      </c>
-      <c r="K60">
+      <c r="I60">
         <v>7.0830000000000002</v>
       </c>
-      <c r="L60">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>45684.438935185186</v>
       </c>
@@ -3197,29 +2645,20 @@
       <c r="E61" t="s">
         <v>64</v>
       </c>
-      <c r="F61">
+      <c r="F61" t="s">
+        <v>123</v>
+      </c>
+      <c r="G61" t="s">
+        <v>126</v>
+      </c>
+      <c r="H61">
         <v>67.5</v>
       </c>
-      <c r="G61">
-        <v>0.78023259259259259</v>
-      </c>
-      <c r="H61" t="s">
-        <v>126</v>
-      </c>
-      <c r="I61" t="s">
-        <v>129</v>
-      </c>
-      <c r="J61">
-        <v>67.5</v>
-      </c>
-      <c r="K61">
+      <c r="I61">
         <v>11.462999999999999</v>
       </c>
-      <c r="L61">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>45684.441319444442</v>
       </c>
@@ -3235,29 +2674,20 @@
       <c r="E62" t="s">
         <v>65</v>
       </c>
-      <c r="F62">
+      <c r="F62" t="s">
+        <v>123</v>
+      </c>
+      <c r="G62" t="s">
+        <v>130</v>
+      </c>
+      <c r="H62">
         <v>36</v>
       </c>
-      <c r="G62">
-        <v>0.56563888888888891</v>
-      </c>
-      <c r="H62" t="s">
-        <v>126</v>
-      </c>
-      <c r="I62" t="s">
-        <v>133</v>
-      </c>
-      <c r="J62">
-        <v>36</v>
-      </c>
-      <c r="K62">
+      <c r="I62">
         <v>7.2380000000000004</v>
       </c>
-      <c r="L62">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>45684.451574074075</v>
       </c>
@@ -3273,29 +2703,20 @@
       <c r="E63" t="s">
         <v>66</v>
       </c>
-      <c r="F63">
+      <c r="F63" t="s">
+        <v>124</v>
+      </c>
+      <c r="G63" t="s">
+        <v>131</v>
+      </c>
+      <c r="H63">
         <v>90</v>
       </c>
-      <c r="G63">
-        <v>0.71564333333333341</v>
-      </c>
-      <c r="H63" t="s">
-        <v>127</v>
-      </c>
-      <c r="I63" t="s">
-        <v>134</v>
-      </c>
-      <c r="J63">
-        <v>90</v>
-      </c>
-      <c r="K63">
+      <c r="I63">
         <v>10.795</v>
       </c>
-      <c r="L63">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>45684.453935185185</v>
       </c>
@@ -3311,29 +2732,20 @@
       <c r="E64" t="s">
         <v>67</v>
       </c>
-      <c r="F64">
+      <c r="F64" t="s">
+        <v>125</v>
+      </c>
+      <c r="G64" t="s">
+        <v>129</v>
+      </c>
+      <c r="H64">
         <v>45</v>
       </c>
-      <c r="G64">
-        <v>0.39249111111111112</v>
-      </c>
-      <c r="H64" t="s">
-        <v>128</v>
-      </c>
-      <c r="I64" t="s">
-        <v>132</v>
-      </c>
-      <c r="J64">
-        <v>45</v>
-      </c>
-      <c r="K64">
+      <c r="I64">
         <v>21.422999999999998</v>
       </c>
-      <c r="L64">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>45684.456817129627</v>
       </c>
@@ -3349,29 +2761,20 @@
       <c r="E65" t="s">
         <v>68</v>
       </c>
-      <c r="F65">
+      <c r="F65" t="s">
+        <v>125</v>
+      </c>
+      <c r="G65" t="s">
+        <v>130</v>
+      </c>
+      <c r="H65">
         <v>44.1</v>
       </c>
-      <c r="G65">
-        <v>0.32596371882086173</v>
-      </c>
-      <c r="H65" t="s">
-        <v>128</v>
-      </c>
-      <c r="I65" t="s">
-        <v>133</v>
-      </c>
-      <c r="J65">
-        <v>44.1</v>
-      </c>
-      <c r="K65">
+      <c r="I65">
         <v>21.609000000000002</v>
       </c>
-      <c r="L65">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>45684.466967592591</v>
       </c>
@@ -3387,29 +2790,20 @@
       <c r="E66" t="s">
         <v>69</v>
       </c>
-      <c r="F66">
+      <c r="F66" t="s">
+        <v>126</v>
+      </c>
+      <c r="G66" t="s">
+        <v>144</v>
+      </c>
+      <c r="H66">
         <v>54.7</v>
       </c>
-      <c r="G66">
-        <v>0.24075319926873862</v>
-      </c>
-      <c r="H66" t="s">
-        <v>129</v>
-      </c>
-      <c r="I66" t="s">
-        <v>147</v>
-      </c>
-      <c r="J66">
-        <v>54.7</v>
-      </c>
-      <c r="K66">
+      <c r="I66">
         <v>20.416</v>
       </c>
-      <c r="L66">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>45684.472384259258</v>
       </c>
@@ -3425,29 +2819,20 @@
       <c r="E67" t="s">
         <v>70</v>
       </c>
-      <c r="F67">
+      <c r="F67" t="s">
+        <v>126</v>
+      </c>
+      <c r="G67" t="s">
+        <v>130</v>
+      </c>
+      <c r="H67">
         <v>54.7</v>
       </c>
-      <c r="G67">
-        <v>0.60016819012797074</v>
-      </c>
-      <c r="H67" t="s">
-        <v>129</v>
-      </c>
-      <c r="I67" t="s">
-        <v>133</v>
-      </c>
-      <c r="J67">
-        <v>54.7</v>
-      </c>
-      <c r="K67">
+      <c r="I67">
         <v>20.273</v>
       </c>
-      <c r="L67">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>45684.47483796296</v>
       </c>
@@ -3463,29 +2848,20 @@
       <c r="E68" t="s">
         <v>71</v>
       </c>
-      <c r="F68">
+      <c r="F68" t="s">
+        <v>127</v>
+      </c>
+      <c r="G68" t="s">
+        <v>141</v>
+      </c>
+      <c r="H68">
         <v>67.5</v>
       </c>
-      <c r="G68">
-        <v>0.20859111111111117</v>
-      </c>
-      <c r="H68" t="s">
-        <v>130</v>
-      </c>
-      <c r="I68" t="s">
-        <v>144</v>
-      </c>
-      <c r="J68">
-        <v>67.5</v>
-      </c>
-      <c r="K68">
+      <c r="I68">
         <v>11.471</v>
       </c>
-      <c r="L68">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>45684.478263888886</v>
       </c>
@@ -3501,29 +2877,20 @@
       <c r="E69" t="s">
         <v>72</v>
       </c>
-      <c r="F69">
+      <c r="F69" t="s">
+        <v>127</v>
+      </c>
+      <c r="G69" t="s">
+        <v>134</v>
+      </c>
+      <c r="H69">
         <v>78.099999999999994</v>
       </c>
-      <c r="G69">
-        <v>0.64793085787451987</v>
-      </c>
-      <c r="H69" t="s">
-        <v>130</v>
-      </c>
-      <c r="I69" t="s">
-        <v>137</v>
-      </c>
-      <c r="J69">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K69">
+      <c r="I69">
         <v>11.919</v>
       </c>
-      <c r="L69">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>45684.480104166665</v>
       </c>
@@ -3539,29 +2906,20 @@
       <c r="E70" t="s">
         <v>73</v>
       </c>
-      <c r="F70">
+      <c r="F70" t="s">
+        <v>127</v>
+      </c>
+      <c r="G70" t="s">
+        <v>147</v>
+      </c>
+      <c r="H70">
         <v>67.5</v>
       </c>
-      <c r="G70">
-        <v>0.33515851851851852</v>
-      </c>
-      <c r="H70" t="s">
-        <v>130</v>
-      </c>
-      <c r="I70" t="s">
-        <v>151</v>
-      </c>
-      <c r="J70">
-        <v>67.5</v>
-      </c>
-      <c r="K70">
+      <c r="I70">
         <v>11.445</v>
       </c>
-      <c r="L70">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>45684.487071759257</v>
       </c>
@@ -3577,29 +2935,20 @@
       <c r="E71" t="s">
         <v>74</v>
       </c>
-      <c r="F71">
+      <c r="F71" t="s">
+        <v>128</v>
+      </c>
+      <c r="G71" t="s">
+        <v>152</v>
+      </c>
+      <c r="H71">
         <v>69.900000000000006</v>
       </c>
-      <c r="G71">
-        <v>0.56055937052932769</v>
-      </c>
-      <c r="H71" t="s">
-        <v>131</v>
-      </c>
-      <c r="I71" t="s">
-        <v>156</v>
-      </c>
-      <c r="J71">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K71">
+      <c r="I71">
         <v>10.468999999999999</v>
       </c>
-      <c r="L71">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>45684.489756944444</v>
       </c>
@@ -3615,29 +2964,20 @@
       <c r="E72" t="s">
         <v>75</v>
       </c>
-      <c r="F72">
+      <c r="F72" t="s">
+        <v>128</v>
+      </c>
+      <c r="G72" t="s">
+        <v>139</v>
+      </c>
+      <c r="H72">
         <v>90</v>
       </c>
-      <c r="G72">
-        <v>0.66763111111111118</v>
-      </c>
-      <c r="H72" t="s">
-        <v>131</v>
-      </c>
-      <c r="I72" t="s">
-        <v>142</v>
-      </c>
-      <c r="J72">
-        <v>90</v>
-      </c>
-      <c r="K72">
+      <c r="I72">
         <v>7.593</v>
       </c>
-      <c r="L72">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>45684.489872685182</v>
       </c>
@@ -3653,29 +2993,20 @@
       <c r="E73" t="s">
         <v>76</v>
       </c>
-      <c r="F73">
+      <c r="F73" t="s">
+        <v>128</v>
+      </c>
+      <c r="G73" t="s">
+        <v>141</v>
+      </c>
+      <c r="H73">
         <v>45</v>
       </c>
-      <c r="G73">
-        <v>0.25800888888888884</v>
-      </c>
-      <c r="H73" t="s">
-        <v>131</v>
-      </c>
-      <c r="I73" t="s">
-        <v>144</v>
-      </c>
-      <c r="J73">
-        <v>45</v>
-      </c>
-      <c r="K73">
+      <c r="I73">
         <v>21.492000000000001</v>
       </c>
-      <c r="L73">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>45684.49722222222</v>
       </c>
@@ -3691,29 +3022,20 @@
       <c r="E74" t="s">
         <v>77</v>
       </c>
-      <c r="F74">
+      <c r="F74" t="s">
+        <v>129</v>
+      </c>
+      <c r="G74" t="s">
+        <v>153</v>
+      </c>
+      <c r="H74">
         <v>78.099999999999994</v>
       </c>
-      <c r="G74">
-        <v>0.54743661971830981</v>
-      </c>
-      <c r="H74" t="s">
-        <v>132</v>
-      </c>
-      <c r="I74" t="s">
-        <v>157</v>
-      </c>
-      <c r="J74">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K74">
+      <c r="I74">
         <v>11.917999999999999</v>
       </c>
-      <c r="L74">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>45684.501967592594</v>
       </c>
@@ -3729,29 +3051,20 @@
       <c r="E75" t="s">
         <v>78</v>
       </c>
-      <c r="F75">
+      <c r="F75" t="s">
+        <v>129</v>
+      </c>
+      <c r="G75" t="s">
+        <v>154</v>
+      </c>
+      <c r="H75">
         <v>45</v>
       </c>
-      <c r="G75">
-        <v>0.5687444444444445</v>
-      </c>
-      <c r="H75" t="s">
-        <v>132</v>
-      </c>
-      <c r="I75" t="s">
-        <v>158</v>
-      </c>
-      <c r="J75">
-        <v>45</v>
-      </c>
-      <c r="K75">
+      <c r="I75">
         <v>21.184999999999999</v>
       </c>
-      <c r="L75">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>45684.50203703704</v>
       </c>
@@ -3767,29 +3080,20 @@
       <c r="E76" t="s">
         <v>79</v>
       </c>
-      <c r="F76">
+      <c r="F76" t="s">
+        <v>129</v>
+      </c>
+      <c r="G76" t="s">
+        <v>155</v>
+      </c>
+      <c r="H76">
         <v>67.5</v>
       </c>
-      <c r="G76">
-        <v>0.41149185185185189</v>
-      </c>
-      <c r="H76" t="s">
-        <v>132</v>
-      </c>
-      <c r="I76" t="s">
-        <v>159</v>
-      </c>
-      <c r="J76">
-        <v>67.5</v>
-      </c>
-      <c r="K76">
+      <c r="I76">
         <v>10.733000000000001</v>
       </c>
-      <c r="L76">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>45684.503148148149</v>
       </c>
@@ -3805,29 +3109,20 @@
       <c r="E77" t="s">
         <v>80</v>
       </c>
-      <c r="F77">
+      <c r="F77" t="s">
+        <v>129</v>
+      </c>
+      <c r="G77" t="s">
+        <v>141</v>
+      </c>
+      <c r="H77">
         <v>90</v>
       </c>
-      <c r="G77">
-        <v>0.62572000000000005</v>
-      </c>
-      <c r="H77" t="s">
-        <v>132</v>
-      </c>
-      <c r="I77" t="s">
-        <v>144</v>
-      </c>
-      <c r="J77">
-        <v>90</v>
-      </c>
-      <c r="K77">
+      <c r="I77">
         <v>7.3920000000000003</v>
       </c>
-      <c r="L77">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>45684.504143518519</v>
       </c>
@@ -3843,29 +3138,20 @@
       <c r="E78" t="s">
         <v>81</v>
       </c>
-      <c r="F78">
+      <c r="F78" t="s">
+        <v>129</v>
+      </c>
+      <c r="G78" t="s">
+        <v>143</v>
+      </c>
+      <c r="H78">
         <v>90</v>
       </c>
-      <c r="G78">
-        <v>0.70002111111111109</v>
-      </c>
-      <c r="H78" t="s">
-        <v>132</v>
-      </c>
-      <c r="I78" t="s">
-        <v>146</v>
-      </c>
-      <c r="J78">
-        <v>90</v>
-      </c>
-      <c r="K78">
+      <c r="I78">
         <v>7.3390000000000004</v>
       </c>
-      <c r="L78">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>45684.505682870367</v>
       </c>
@@ -3881,29 +3167,20 @@
       <c r="E79" t="s">
         <v>82</v>
       </c>
-      <c r="F79">
+      <c r="F79" t="s">
+        <v>130</v>
+      </c>
+      <c r="G79" t="s">
+        <v>156</v>
+      </c>
+      <c r="H79">
         <v>90</v>
       </c>
-      <c r="G79">
-        <v>0.69203222222222227</v>
-      </c>
-      <c r="H79" t="s">
-        <v>133</v>
-      </c>
-      <c r="I79" t="s">
-        <v>160</v>
-      </c>
-      <c r="J79">
-        <v>90</v>
-      </c>
-      <c r="K79">
+      <c r="I79">
         <v>7.7720000000000002</v>
       </c>
-      <c r="L79">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>45684.506851851853</v>
       </c>
@@ -3919,29 +3196,20 @@
       <c r="E80" t="s">
         <v>83</v>
       </c>
-      <c r="F80">
+      <c r="F80" t="s">
+        <v>130</v>
+      </c>
+      <c r="G80" t="s">
+        <v>153</v>
+      </c>
+      <c r="H80">
         <v>54.7</v>
       </c>
-      <c r="G80">
-        <v>0.6786252285191956</v>
-      </c>
-      <c r="H80" t="s">
-        <v>133</v>
-      </c>
-      <c r="I80" t="s">
-        <v>157</v>
-      </c>
-      <c r="J80">
-        <v>54.7</v>
-      </c>
-      <c r="K80">
+      <c r="I80">
         <v>20.033999999999999</v>
       </c>
-      <c r="L80">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>45684.513402777775</v>
       </c>
@@ -3957,29 +3225,20 @@
       <c r="E81" t="s">
         <v>84</v>
       </c>
-      <c r="F81">
+      <c r="F81" t="s">
+        <v>130</v>
+      </c>
+      <c r="G81" t="s">
+        <v>157</v>
+      </c>
+      <c r="H81">
         <v>90</v>
       </c>
-      <c r="G81">
-        <v>0.66811888888888893</v>
-      </c>
-      <c r="H81" t="s">
-        <v>133</v>
-      </c>
-      <c r="I81" t="s">
-        <v>161</v>
-      </c>
-      <c r="J81">
-        <v>90</v>
-      </c>
-      <c r="K81">
+      <c r="I81">
         <v>7.9029999999999996</v>
       </c>
-      <c r="L81">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>45684.517025462963</v>
       </c>
@@ -3995,29 +3254,20 @@
       <c r="E82" t="s">
         <v>85</v>
       </c>
-      <c r="F82">
+      <c r="F82" t="s">
+        <v>131</v>
+      </c>
+      <c r="G82" t="s">
+        <v>140</v>
+      </c>
+      <c r="H82">
         <v>69.900000000000006</v>
       </c>
-      <c r="G82">
-        <v>0.70748927038626608</v>
-      </c>
-      <c r="H82" t="s">
-        <v>134</v>
-      </c>
-      <c r="I82" t="s">
-        <v>143</v>
-      </c>
-      <c r="J82">
-        <v>69.900000000000006</v>
-      </c>
-      <c r="K82">
+      <c r="I82">
         <v>10.577</v>
       </c>
-      <c r="L82">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>45684.523425925923</v>
       </c>
@@ -4033,29 +3283,20 @@
       <c r="E83" t="s">
         <v>86</v>
       </c>
-      <c r="F83">
+      <c r="F83" t="s">
+        <v>131</v>
+      </c>
+      <c r="G83" t="s">
+        <v>141</v>
+      </c>
+      <c r="H83">
         <v>54.7</v>
       </c>
-      <c r="G83">
-        <v>0.57453016453382089</v>
-      </c>
-      <c r="H83" t="s">
-        <v>134</v>
-      </c>
-      <c r="I83" t="s">
-        <v>144</v>
-      </c>
-      <c r="J83">
-        <v>54.7</v>
-      </c>
-      <c r="K83">
+      <c r="I83">
         <v>20.664000000000001</v>
       </c>
-      <c r="L83">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>45684.525567129633</v>
       </c>
@@ -4071,29 +3312,20 @@
       <c r="E84" t="s">
         <v>87</v>
       </c>
-      <c r="F84">
+      <c r="F84" t="s">
+        <v>131</v>
+      </c>
+      <c r="G84" t="s">
+        <v>141</v>
+      </c>
+      <c r="H84">
         <v>90</v>
       </c>
-      <c r="G84">
-        <v>0.85476444444444444</v>
-      </c>
-      <c r="H84" t="s">
-        <v>134</v>
-      </c>
-      <c r="I84" t="s">
-        <v>144</v>
-      </c>
-      <c r="J84">
-        <v>90</v>
-      </c>
-      <c r="K84">
+      <c r="I84">
         <v>7.3780000000000001</v>
       </c>
-      <c r="L84">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>45684.525787037041</v>
       </c>
@@ -4109,29 +3341,20 @@
       <c r="E85" t="s">
         <v>88</v>
       </c>
-      <c r="F85">
+      <c r="F85" t="s">
+        <v>131</v>
+      </c>
+      <c r="G85" t="s">
+        <v>136</v>
+      </c>
+      <c r="H85">
         <v>78.099999999999994</v>
       </c>
-      <c r="G85">
-        <v>0.74978233034571062</v>
-      </c>
-      <c r="H85" t="s">
-        <v>134</v>
-      </c>
-      <c r="I85" t="s">
-        <v>139</v>
-      </c>
-      <c r="J85">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K85">
+      <c r="I85">
         <v>11.624000000000001</v>
       </c>
-      <c r="L85">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>45684.529895833337</v>
       </c>
@@ -4147,29 +3370,20 @@
       <c r="E86" t="s">
         <v>89</v>
       </c>
-      <c r="F86">
+      <c r="F86" t="s">
+        <v>132</v>
+      </c>
+      <c r="G86" t="s">
+        <v>157</v>
+      </c>
+      <c r="H86">
         <v>54.7</v>
       </c>
-      <c r="G86">
-        <v>4.966361974405864E-2</v>
-      </c>
-      <c r="H86" t="s">
-        <v>135</v>
-      </c>
-      <c r="I86" t="s">
-        <v>161</v>
-      </c>
-      <c r="J86">
-        <v>54.7</v>
-      </c>
-      <c r="K86">
+      <c r="I86">
         <v>20.102</v>
       </c>
-      <c r="L86">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>45684.540486111109</v>
       </c>
@@ -4185,29 +3399,20 @@
       <c r="E87" t="s">
         <v>90</v>
       </c>
-      <c r="F87">
+      <c r="F87" t="s">
+        <v>133</v>
+      </c>
+      <c r="G87" t="s">
+        <v>143</v>
+      </c>
+      <c r="H87">
         <v>62</v>
       </c>
-      <c r="G87">
-        <v>0.672341935483871</v>
-      </c>
-      <c r="H87" t="s">
-        <v>136</v>
-      </c>
-      <c r="I87" t="s">
-        <v>146</v>
-      </c>
-      <c r="J87">
-        <v>62</v>
-      </c>
-      <c r="K87">
+      <c r="I87">
         <v>6.6630000000000003</v>
       </c>
-      <c r="L87">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>45684.545671296299</v>
       </c>
@@ -4223,29 +3428,20 @@
       <c r="E88" t="s">
         <v>91</v>
       </c>
-      <c r="F88">
+      <c r="F88" t="s">
+        <v>133</v>
+      </c>
+      <c r="G88" t="s">
+        <v>140</v>
+      </c>
+      <c r="H88">
         <v>82</v>
       </c>
-      <c r="G88">
-        <v>0.74890609756097559</v>
-      </c>
-      <c r="H88" t="s">
-        <v>136</v>
-      </c>
-      <c r="I88" t="s">
-        <v>143</v>
-      </c>
-      <c r="J88">
-        <v>82</v>
-      </c>
-      <c r="K88">
+      <c r="I88">
         <v>11.013999999999999</v>
       </c>
-      <c r="L88">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>45684.547905092593</v>
       </c>
@@ -4261,29 +3457,20 @@
       <c r="E89" t="s">
         <v>92</v>
       </c>
-      <c r="F89">
+      <c r="F89" t="s">
+        <v>134</v>
+      </c>
+      <c r="G89" t="s">
+        <v>142</v>
+      </c>
+      <c r="H89">
         <v>47.342111111111109</v>
       </c>
-      <c r="G89">
-        <v>0</v>
-      </c>
-      <c r="H89" t="s">
-        <v>137</v>
-      </c>
-      <c r="I89" t="s">
-        <v>145</v>
-      </c>
-      <c r="J89">
-        <v>47.342111111111109</v>
-      </c>
-      <c r="K89">
+      <c r="I89">
         <v>21.605</v>
       </c>
-      <c r="L89">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>45684.548159722224</v>
       </c>
@@ -4299,29 +3486,20 @@
       <c r="E90" t="s">
         <v>93</v>
       </c>
-      <c r="F90">
+      <c r="F90" t="s">
+        <v>134</v>
+      </c>
+      <c r="G90" t="s">
+        <v>157</v>
+      </c>
+      <c r="H90">
         <v>40</v>
       </c>
-      <c r="G90">
-        <v>0.4248575</v>
-      </c>
-      <c r="H90" t="s">
-        <v>137</v>
-      </c>
-      <c r="I90" t="s">
-        <v>161</v>
-      </c>
-      <c r="J90">
-        <v>40</v>
-      </c>
-      <c r="K90">
+      <c r="I90">
         <v>6.9720000000000004</v>
       </c>
-      <c r="L90">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>45684.556817129633</v>
       </c>
@@ -4337,29 +3515,20 @@
       <c r="E91" t="s">
         <v>94</v>
       </c>
-      <c r="F91">
+      <c r="F91" t="s">
+        <v>134</v>
+      </c>
+      <c r="G91" t="s">
+        <v>150</v>
+      </c>
+      <c r="H91">
         <v>90</v>
       </c>
-      <c r="G91">
-        <v>0.82498777777777776</v>
-      </c>
-      <c r="H91" t="s">
-        <v>137</v>
-      </c>
-      <c r="I91" t="s">
-        <v>154</v>
-      </c>
-      <c r="J91">
-        <v>90</v>
-      </c>
-      <c r="K91">
+      <c r="I91">
         <v>7.4960000000000004</v>
       </c>
-      <c r="L91">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>45684.567627314813</v>
       </c>
@@ -4375,29 +3544,20 @@
       <c r="E92" t="s">
         <v>95</v>
       </c>
-      <c r="F92">
+      <c r="F92" t="s">
+        <v>135</v>
+      </c>
+      <c r="G92" t="s">
+        <v>141</v>
+      </c>
+      <c r="H92">
         <v>90</v>
       </c>
-      <c r="G92">
-        <v>0.75327444444444447</v>
-      </c>
-      <c r="H92" t="s">
-        <v>138</v>
-      </c>
-      <c r="I92" t="s">
-        <v>144</v>
-      </c>
-      <c r="J92">
-        <v>90</v>
-      </c>
-      <c r="K92">
+      <c r="I92">
         <v>7.6479999999999997</v>
       </c>
-      <c r="L92">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>45684.57503472222</v>
       </c>
@@ -4413,29 +3573,20 @@
       <c r="E93" t="s">
         <v>96</v>
       </c>
-      <c r="F93">
+      <c r="F93" t="s">
+        <v>136</v>
+      </c>
+      <c r="G93" t="s">
+        <v>139</v>
+      </c>
+      <c r="H93">
         <v>78.099999999999994</v>
       </c>
-      <c r="G93">
-        <v>0.81925864276568505</v>
-      </c>
-      <c r="H93" t="s">
-        <v>139</v>
-      </c>
-      <c r="I93" t="s">
-        <v>142</v>
-      </c>
-      <c r="J93">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K93">
+      <c r="I93">
         <v>11.756</v>
       </c>
-      <c r="L93">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>45684.581689814811</v>
       </c>
@@ -4451,29 +3602,20 @@
       <c r="E94" t="s">
         <v>97</v>
       </c>
-      <c r="F94">
+      <c r="F94" t="s">
+        <v>137</v>
+      </c>
+      <c r="G94" t="s">
+        <v>140</v>
+      </c>
+      <c r="H94">
         <v>36</v>
       </c>
-      <c r="G94">
-        <v>0.63976666666666671</v>
-      </c>
-      <c r="H94" t="s">
-        <v>140</v>
-      </c>
-      <c r="I94" t="s">
-        <v>143</v>
-      </c>
-      <c r="J94">
-        <v>36</v>
-      </c>
-      <c r="K94">
+      <c r="I94">
         <v>7.24</v>
       </c>
-      <c r="L94">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>45684.594201388885</v>
       </c>
@@ -4489,29 +3631,20 @@
       <c r="E95" t="s">
         <v>98</v>
       </c>
-      <c r="F95">
+      <c r="F95" t="s">
+        <v>138</v>
+      </c>
+      <c r="G95" t="s">
+        <v>152</v>
+      </c>
+      <c r="H95">
         <v>62</v>
       </c>
-      <c r="G95">
-        <v>0.84061935483870975</v>
-      </c>
-      <c r="H95" t="s">
-        <v>141</v>
-      </c>
-      <c r="I95" t="s">
-        <v>156</v>
-      </c>
-      <c r="J95">
-        <v>62</v>
-      </c>
-      <c r="K95">
+      <c r="I95">
         <v>6.3529999999999998</v>
       </c>
-      <c r="L95">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>45684.616655092592</v>
       </c>
@@ -4527,29 +3660,20 @@
       <c r="E96" t="s">
         <v>99</v>
       </c>
-      <c r="F96">
+      <c r="F96" t="s">
+        <v>139</v>
+      </c>
+      <c r="G96" t="s">
+        <v>157</v>
+      </c>
+      <c r="H96">
         <v>90</v>
       </c>
-      <c r="G96">
-        <v>0.79439111111111116</v>
-      </c>
-      <c r="H96" t="s">
-        <v>142</v>
-      </c>
-      <c r="I96" t="s">
-        <v>161</v>
-      </c>
-      <c r="J96">
-        <v>90</v>
-      </c>
-      <c r="K96">
+      <c r="I96">
         <v>7.6029999999999998</v>
       </c>
-      <c r="L96">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>45684.639270833337</v>
       </c>
@@ -4565,29 +3689,20 @@
       <c r="E97" t="s">
         <v>100</v>
       </c>
-      <c r="F97">
+      <c r="F97" t="s">
+        <v>140</v>
+      </c>
+      <c r="G97" t="s">
+        <v>151</v>
+      </c>
+      <c r="H97">
         <v>67.5</v>
       </c>
-      <c r="G97">
-        <v>0.73306666666666664</v>
-      </c>
-      <c r="H97" t="s">
-        <v>143</v>
-      </c>
-      <c r="I97" t="s">
-        <v>155</v>
-      </c>
-      <c r="J97">
-        <v>67.5</v>
-      </c>
-      <c r="K97">
+      <c r="I97">
         <v>10.711</v>
       </c>
-      <c r="L97">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>45684.642476851855</v>
       </c>
@@ -4603,29 +3718,20 @@
       <c r="E98" t="s">
         <v>101</v>
       </c>
-      <c r="F98">
+      <c r="F98" t="s">
+        <v>141</v>
+      </c>
+      <c r="G98" t="s">
+        <v>156</v>
+      </c>
+      <c r="H98">
         <v>90</v>
       </c>
-      <c r="G98">
-        <v>0.88943000000000005</v>
-      </c>
-      <c r="H98" t="s">
-        <v>144</v>
-      </c>
-      <c r="I98" t="s">
-        <v>160</v>
-      </c>
-      <c r="J98">
-        <v>90</v>
-      </c>
-      <c r="K98">
+      <c r="I98">
         <v>7.3369999999999997</v>
       </c>
-      <c r="L98">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>45684.642488425925</v>
       </c>
@@ -4641,29 +3747,20 @@
       <c r="E99" t="s">
         <v>102</v>
       </c>
-      <c r="F99">
+      <c r="F99" t="s">
+        <v>141</v>
+      </c>
+      <c r="G99" t="s">
+        <v>156</v>
+      </c>
+      <c r="H99">
         <v>90</v>
       </c>
-      <c r="G99">
-        <v>0.83375555555555558</v>
-      </c>
-      <c r="H99" t="s">
-        <v>144</v>
-      </c>
-      <c r="I99" t="s">
-        <v>160</v>
-      </c>
-      <c r="J99">
-        <v>90</v>
-      </c>
-      <c r="K99">
+      <c r="I99">
         <v>7.5890000000000004</v>
       </c>
-      <c r="L99">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>45684.655648148146</v>
       </c>
@@ -4679,29 +3776,20 @@
       <c r="E100" t="s">
         <v>103</v>
       </c>
-      <c r="F100">
+      <c r="F100" t="s">
+        <v>142</v>
+      </c>
+      <c r="G100" t="s">
+        <v>145</v>
+      </c>
+      <c r="H100">
         <v>78.099999999999994</v>
       </c>
-      <c r="G100">
-        <v>0.60201280409731117</v>
-      </c>
-      <c r="H100" t="s">
-        <v>145</v>
-      </c>
-      <c r="I100" t="s">
-        <v>148</v>
-      </c>
-      <c r="J100">
-        <v>78.099999999999994</v>
-      </c>
-      <c r="K100">
+      <c r="I100">
         <v>11.638999999999999</v>
       </c>
-      <c r="L100">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>45684.660300925927</v>
       </c>
@@ -4717,29 +3805,20 @@
       <c r="E101" t="s">
         <v>104</v>
       </c>
-      <c r="F101">
+      <c r="F101" t="s">
+        <v>142</v>
+      </c>
+      <c r="G101" t="s">
+        <v>151</v>
+      </c>
+      <c r="H101">
         <v>90</v>
       </c>
-      <c r="G101">
-        <v>0.85714777777777784</v>
-      </c>
-      <c r="H101" t="s">
-        <v>145</v>
-      </c>
-      <c r="I101" t="s">
-        <v>155</v>
-      </c>
-      <c r="J101">
-        <v>90</v>
-      </c>
-      <c r="K101">
+      <c r="I101">
         <v>7.52</v>
       </c>
-      <c r="L101">
-        <v>1.44</v>
-      </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>45684.694745370369</v>
       </c>
@@ -4755,29 +3834,20 @@
       <c r="E102" t="s">
         <v>105</v>
       </c>
-      <c r="F102">
+      <c r="F102" t="s">
+        <v>143</v>
+      </c>
+      <c r="G102" t="s">
+        <v>158</v>
+      </c>
+      <c r="H102">
         <v>54.7</v>
       </c>
-      <c r="G102">
-        <v>0.60793967093235834</v>
-      </c>
-      <c r="H102" t="s">
-        <v>146</v>
-      </c>
-      <c r="I102" t="s">
-        <v>162</v>
-      </c>
-      <c r="J102">
-        <v>54.7</v>
-      </c>
-      <c r="K102">
+      <c r="I102">
         <v>20.558</v>
       </c>
-      <c r="L102">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>45684.720937500002</v>
       </c>
@@ -4793,29 +3863,20 @@
       <c r="E103" t="s">
         <v>106</v>
       </c>
-      <c r="F103">
+      <c r="F103" t="s">
+        <v>144</v>
+      </c>
+      <c r="G103" t="s">
+        <v>159</v>
+      </c>
+      <c r="H103">
         <v>45</v>
       </c>
-      <c r="G103">
-        <v>0.12199333333333329</v>
-      </c>
-      <c r="H103" t="s">
-        <v>147</v>
-      </c>
-      <c r="I103" t="s">
-        <v>163</v>
-      </c>
-      <c r="J103">
-        <v>45</v>
-      </c>
-      <c r="K103">
+      <c r="I103">
         <v>21.579000000000001</v>
       </c>
-      <c r="L103">
-        <v>4.32</v>
-      </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>45684.736331018517</v>
       </c>
@@ -4831,26 +3892,17 @@
       <c r="E104" t="s">
         <v>107</v>
       </c>
-      <c r="F104">
+      <c r="F104" t="s">
+        <v>145</v>
+      </c>
+      <c r="G104" t="s">
+        <v>160</v>
+      </c>
+      <c r="H104">
         <v>90</v>
       </c>
-      <c r="G104">
-        <v>0.79518222222222223</v>
-      </c>
-      <c r="H104" t="s">
-        <v>148</v>
-      </c>
-      <c r="I104" t="s">
-        <v>164</v>
-      </c>
-      <c r="J104">
-        <v>90</v>
-      </c>
-      <c r="K104">
+      <c r="I104">
         <v>7.2830000000000004</v>
-      </c>
-      <c r="L104">
-        <v>1.44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>